<commit_message>
Added Single Transferable Vote
</commit_message>
<xml_diff>
--- a/Grad Clothing voting/ballots_table.xlsx
+++ b/Grad Clothing voting/ballots_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABEACE02ECD4E35F4CB25BDE589F" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B8F63E25-46D8-4213-8794-7B357ECD0CB8}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABEACE02ECD4E35F4CB25BDE589F" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{A0E4D1E1-9641-41A2-841F-DC359DE45589}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Email Address</t>
   </si>
@@ -254,6 +254,54 @@
   </si>
   <si>
     <t>linje@utschools.ca</t>
+  </si>
+  <si>
+    <t>hanst@utschools.ca</t>
+  </si>
+  <si>
+    <t>thave@utschools.ca</t>
+  </si>
+  <si>
+    <t>onesh@utschools.ca</t>
+  </si>
+  <si>
+    <t>chakr@utschools.ca</t>
+  </si>
+  <si>
+    <t>zhora@utschools.ca</t>
+  </si>
+  <si>
+    <t>leejo@utschools.ca</t>
+  </si>
+  <si>
+    <t>tench@utschools.ca</t>
+  </si>
+  <si>
+    <t>leesun@utschools.ca</t>
+  </si>
+  <si>
+    <t>jinbe@utschools.ca</t>
+  </si>
+  <si>
+    <t>mohma@utschools.ca</t>
+  </si>
+  <si>
+    <t>liuann@utschools.ca</t>
+  </si>
+  <si>
+    <t>winar@utschools.ca</t>
+  </si>
+  <si>
+    <t>linda@utschools.ca</t>
+  </si>
+  <si>
+    <t>huaei@utschools.ca</t>
+  </si>
+  <si>
+    <t>pfesa@utschools.ca</t>
+  </si>
+  <si>
+    <t>wanma@utschools.ca</t>
   </si>
 </sst>
 </file>
@@ -583,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S160"/>
+  <dimension ref="A1:S176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3405,71 +3453,147 @@
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+    <row r="61" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="2">
+        <v>7</v>
+      </c>
+      <c r="C61" s="2">
+        <v>3</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
       <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="H61" s="2">
+        <v>4</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
+      <c r="M61" s="2">
+        <v>5</v>
+      </c>
+      <c r="N61" s="2">
+        <v>8</v>
+      </c>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
+      <c r="Q61" s="2">
+        <v>9</v>
+      </c>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+    <row r="62" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="2">
+        <v>9</v>
+      </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
+      <c r="I62" s="2">
+        <v>1</v>
+      </c>
+      <c r="J62" s="2">
+        <v>6</v>
+      </c>
+      <c r="K62" s="2">
+        <v>5</v>
+      </c>
+      <c r="L62" s="2">
+        <v>4</v>
+      </c>
       <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
+      <c r="N62" s="2">
+        <v>7</v>
+      </c>
+      <c r="O62" s="2">
+        <v>3</v>
+      </c>
+      <c r="P62" s="2">
+        <v>2</v>
+      </c>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="R62" s="2">
+        <v>8</v>
+      </c>
       <c r="S62" s="1"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
+    <row r="63" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="2">
+        <v>2</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3</v>
+      </c>
+      <c r="D63" s="2">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2">
+        <v>16</v>
+      </c>
+      <c r="F63" s="2">
+        <v>4</v>
+      </c>
+      <c r="G63" s="2">
+        <v>17</v>
+      </c>
+      <c r="H63" s="2">
+        <v>5</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="2">
+        <v>12</v>
+      </c>
+      <c r="K63" s="2">
+        <v>10</v>
+      </c>
+      <c r="L63" s="2">
+        <v>18</v>
+      </c>
       <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A64" s="1"/>
+      <c r="N63" s="2">
+        <v>11</v>
+      </c>
+      <c r="O63" s="2">
+        <v>8</v>
+      </c>
+      <c r="P63" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>14</v>
+      </c>
+      <c r="R63" s="2">
+        <v>15</v>
+      </c>
+      <c r="S63" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3486,33 +3610,63 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="R64" s="2">
+        <v>2</v>
+      </c>
+      <c r="S64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="2">
+        <v>2</v>
+      </c>
+      <c r="C65" s="2">
+        <v>8</v>
+      </c>
+      <c r="D65" s="2">
+        <v>10</v>
+      </c>
+      <c r="E65" s="2">
+        <v>3</v>
+      </c>
+      <c r="F65" s="2">
+        <v>11</v>
+      </c>
       <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="H65" s="2">
+        <v>12</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
+      <c r="M65" s="2">
+        <v>9</v>
+      </c>
+      <c r="N65" s="2">
+        <v>1</v>
+      </c>
+      <c r="O65" s="2">
+        <v>5</v>
+      </c>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="S65" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3521,21 +3675,33 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
+      <c r="K66" s="2">
+        <v>3</v>
+      </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
+      <c r="N66" s="2">
+        <v>1</v>
+      </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
+      <c r="Q66" s="2">
+        <v>4</v>
+      </c>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+    <row r="67" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="2">
+        <v>3</v>
+      </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3544,128 +3710,288 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
+      <c r="M67" s="2">
+        <v>2</v>
+      </c>
+      <c r="N67" s="2">
+        <v>4</v>
+      </c>
+      <c r="O67" s="2">
+        <v>5</v>
+      </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="S67" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="2">
+        <v>17</v>
+      </c>
+      <c r="C68" s="2">
+        <v>16</v>
+      </c>
+      <c r="D68" s="2">
+        <v>15</v>
+      </c>
+      <c r="E68" s="2">
+        <v>14</v>
+      </c>
+      <c r="F68" s="2">
+        <v>13</v>
+      </c>
+      <c r="G68" s="2">
+        <v>12</v>
+      </c>
+      <c r="H68" s="2">
+        <v>11</v>
+      </c>
+      <c r="I68" s="2">
+        <v>10</v>
+      </c>
+      <c r="J68" s="2">
+        <v>9</v>
+      </c>
+      <c r="K68" s="2">
+        <v>8</v>
+      </c>
+      <c r="L68" s="2">
+        <v>7</v>
+      </c>
+      <c r="M68" s="2">
+        <v>6</v>
+      </c>
+      <c r="N68" s="2">
+        <v>18</v>
+      </c>
+      <c r="O68" s="2">
+        <v>5</v>
+      </c>
+      <c r="P68" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>3</v>
+      </c>
+      <c r="R68" s="2">
+        <v>2</v>
+      </c>
+      <c r="S68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2</v>
+      </c>
+      <c r="D69" s="2">
+        <v>13</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
+      <c r="G69" s="2">
+        <v>18</v>
+      </c>
+      <c r="H69" s="2">
+        <v>14</v>
+      </c>
+      <c r="I69" s="2">
+        <v>15</v>
+      </c>
+      <c r="J69" s="2">
+        <v>17</v>
+      </c>
       <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
+      <c r="L69" s="2">
+        <v>16</v>
+      </c>
+      <c r="M69" s="2">
+        <v>12</v>
+      </c>
+      <c r="N69" s="2">
+        <v>5</v>
+      </c>
+      <c r="O69" s="2">
+        <v>3</v>
+      </c>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A71" s="1"/>
+      <c r="S69" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="2">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2">
+        <v>13</v>
+      </c>
+      <c r="D70" s="2">
+        <v>8</v>
+      </c>
+      <c r="E70" s="2">
+        <v>11</v>
+      </c>
+      <c r="F70" s="2">
+        <v>7</v>
+      </c>
+      <c r="G70" s="2">
+        <v>12</v>
+      </c>
+      <c r="H70" s="2">
+        <v>4</v>
+      </c>
+      <c r="I70" s="2">
+        <v>3</v>
+      </c>
+      <c r="J70" s="2">
+        <v>15</v>
+      </c>
+      <c r="K70" s="2">
+        <v>16</v>
+      </c>
+      <c r="L70" s="2">
+        <v>2</v>
+      </c>
+      <c r="M70" s="2">
+        <v>9</v>
+      </c>
+      <c r="N70" s="2">
+        <v>5</v>
+      </c>
+      <c r="O70" s="2">
+        <v>1</v>
+      </c>
+      <c r="P70" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>17</v>
+      </c>
+      <c r="R70" s="2">
+        <v>18</v>
+      </c>
+      <c r="S70" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2">
+        <v>5</v>
+      </c>
+      <c r="E71" s="2">
+        <v>17</v>
+      </c>
+      <c r="F71" s="2">
+        <v>3</v>
+      </c>
+      <c r="G71" s="2">
+        <v>18</v>
+      </c>
       <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
+      <c r="I71" s="2">
+        <v>4</v>
+      </c>
       <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
+      <c r="K71" s="2">
+        <v>14</v>
+      </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
+      <c r="N71" s="2">
+        <v>2</v>
+      </c>
+      <c r="O71" s="2">
+        <v>16</v>
+      </c>
       <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
+      <c r="Q71" s="2">
+        <v>15</v>
+      </c>
       <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A72" s="1"/>
+      <c r="S71" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+      <c r="D72" s="2">
+        <v>5</v>
+      </c>
+      <c r="E72" s="2">
+        <v>6</v>
+      </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
+      <c r="J72" s="2">
+        <v>2</v>
+      </c>
       <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
+      <c r="L72" s="2">
+        <v>7</v>
+      </c>
       <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
+      <c r="N72" s="2">
+        <v>4</v>
+      </c>
+      <c r="O72" s="2">
+        <v>3</v>
+      </c>
+      <c r="P72" s="2">
+        <v>1</v>
+      </c>
       <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A73" s="1"/>
+      <c r="R72" s="2">
+        <v>8</v>
+      </c>
+      <c r="S72" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="C73" s="2">
+        <v>2</v>
+      </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3676,10 +4002,14 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A74" s="1"/>
+      <c r="S73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3699,45 +4029,85 @@
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A75" s="1"/>
+    <row r="75" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
+      <c r="G75" s="2">
+        <v>6</v>
+      </c>
+      <c r="H75" s="2">
+        <v>8</v>
+      </c>
+      <c r="I75" s="2">
+        <v>5</v>
+      </c>
+      <c r="J75" s="2">
+        <v>1</v>
+      </c>
       <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
+      <c r="L75" s="2">
+        <v>3</v>
+      </c>
+      <c r="M75" s="2">
+        <v>9</v>
+      </c>
       <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
+      <c r="O75" s="2">
+        <v>4</v>
+      </c>
+      <c r="P75" s="2">
+        <v>2</v>
+      </c>
       <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
+      <c r="R75" s="2">
+        <v>7</v>
+      </c>
       <c r="S75" s="1"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+    <row r="76" spans="1:19" ht="39" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="2">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2">
+        <v>5</v>
+      </c>
       <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
+      <c r="E76" s="2">
+        <v>2</v>
+      </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
+      <c r="I76" s="2">
+        <v>4</v>
+      </c>
       <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
+      <c r="K76" s="2">
+        <v>6</v>
+      </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
+      <c r="N76" s="2">
+        <v>1</v>
+      </c>
+      <c r="O76" s="2">
+        <v>7</v>
+      </c>
+      <c r="P76" s="2">
+        <v>9</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>8</v>
+      </c>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
     </row>
@@ -5505,6 +5875,342 @@
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
     </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+      <c r="O161" s="1"/>
+      <c r="P161" s="1"/>
+      <c r="Q161" s="1"/>
+      <c r="R161" s="1"/>
+      <c r="S161" s="1"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+      <c r="N162" s="1"/>
+      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
+      <c r="Q162" s="1"/>
+      <c r="R162" s="1"/>
+      <c r="S162" s="1"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
+      <c r="I163" s="1"/>
+      <c r="J163" s="1"/>
+      <c r="K163" s="1"/>
+      <c r="L163" s="1"/>
+      <c r="M163" s="1"/>
+      <c r="N163" s="1"/>
+      <c r="O163" s="1"/>
+      <c r="P163" s="1"/>
+      <c r="Q163" s="1"/>
+      <c r="R163" s="1"/>
+      <c r="S163" s="1"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+      <c r="L164" s="1"/>
+      <c r="M164" s="1"/>
+      <c r="N164" s="1"/>
+      <c r="O164" s="1"/>
+      <c r="P164" s="1"/>
+      <c r="Q164" s="1"/>
+      <c r="R164" s="1"/>
+      <c r="S164" s="1"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1"/>
+      <c r="I165" s="1"/>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+      <c r="L165" s="1"/>
+      <c r="M165" s="1"/>
+      <c r="N165" s="1"/>
+      <c r="O165" s="1"/>
+      <c r="P165" s="1"/>
+      <c r="Q165" s="1"/>
+      <c r="R165" s="1"/>
+      <c r="S165" s="1"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1"/>
+      <c r="I166" s="1"/>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+      <c r="L166" s="1"/>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
+      <c r="O166" s="1"/>
+      <c r="P166" s="1"/>
+      <c r="Q166" s="1"/>
+      <c r="R166" s="1"/>
+      <c r="S166" s="1"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+      <c r="L167" s="1"/>
+      <c r="M167" s="1"/>
+      <c r="N167" s="1"/>
+      <c r="O167" s="1"/>
+      <c r="P167" s="1"/>
+      <c r="Q167" s="1"/>
+      <c r="R167" s="1"/>
+      <c r="S167" s="1"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
+      <c r="Q168" s="1"/>
+      <c r="R168" s="1"/>
+      <c r="S168" s="1"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+      <c r="N169" s="1"/>
+      <c r="O169" s="1"/>
+      <c r="P169" s="1"/>
+      <c r="Q169" s="1"/>
+      <c r="R169" s="1"/>
+      <c r="S169" s="1"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+      <c r="N170" s="1"/>
+      <c r="O170" s="1"/>
+      <c r="P170" s="1"/>
+      <c r="Q170" s="1"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="M171" s="1"/>
+      <c r="N171" s="1"/>
+      <c r="O171" s="1"/>
+      <c r="P171" s="1"/>
+      <c r="Q171" s="1"/>
+      <c r="R171" s="1"/>
+      <c r="S171" s="1"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="1"/>
+      <c r="N172" s="1"/>
+      <c r="O172" s="1"/>
+      <c r="P172" s="1"/>
+      <c r="Q172" s="1"/>
+      <c r="R172" s="1"/>
+      <c r="S172" s="1"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
+      <c r="N173" s="1"/>
+      <c r="O173" s="1"/>
+      <c r="P173" s="1"/>
+      <c r="Q173" s="1"/>
+      <c r="R173" s="1"/>
+      <c r="S173" s="1"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
+      <c r="I174" s="1"/>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+      <c r="L174" s="1"/>
+      <c r="M174" s="1"/>
+      <c r="N174" s="1"/>
+      <c r="O174" s="1"/>
+      <c r="P174" s="1"/>
+      <c r="Q174" s="1"/>
+      <c r="R174" s="1"/>
+      <c r="S174" s="1"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="1"/>
+      <c r="N175" s="1"/>
+      <c r="O175" s="1"/>
+      <c r="P175" s="1"/>
+      <c r="Q175" s="1"/>
+      <c r="R175" s="1"/>
+      <c r="S175" s="1"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
+      <c r="Q176" s="1"/>
+      <c r="R176" s="1"/>
+      <c r="S176" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>